<commit_message>
Added changes for tank pres and feed pres
</commit_message>
<xml_diff>
--- a/Graphs/feed_temp_sweep_results.xlsx
+++ b/Graphs/feed_temp_sweep_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="36" uniqueCount="9">
   <si>
     <t>LH2 Feed temperature (K)</t>
   </si>
@@ -91,15 +91,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="true"/>
-    <col min="2" max="2" width="33.28515625" customWidth="true"/>
-    <col min="3" max="3" width="31.85546875" customWidth="true"/>
-    <col min="4" max="4" width="38.7109375" customWidth="true"/>
-    <col min="5" max="5" width="32" customWidth="true"/>
-    <col min="6" max="6" width="30.5703125" customWidth="true"/>
-    <col min="7" max="7" width="37.42578125" customWidth="true"/>
-    <col min="8" max="8" width="32.28515625" customWidth="true"/>
-    <col min="9" max="9" width="31" customWidth="true"/>
+    <col min="1" max="1" width="21.59765625" customWidth="true"/>
+    <col min="2" max="2" width="30.265625" customWidth="true"/>
+    <col min="3" max="3" width="28.86328125" customWidth="true"/>
+    <col min="4" max="4" width="35.19921875" customWidth="true"/>
+    <col min="5" max="5" width="29" customWidth="true"/>
+    <col min="6" max="6" width="27.59765625" customWidth="true"/>
+    <col min="7" max="7" width="33.9296875" customWidth="true"/>
+    <col min="8" max="8" width="29.19921875" customWidth="true"/>
+    <col min="9" max="9" width="27.9296875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -133,89 +133,89 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>18.333333333333332</v>
+        <v>0.01</v>
       </c>
       <c r="B2" s="0">
-        <v>33.236916680673971</v>
+        <v>32.447837977294029</v>
       </c>
       <c r="C2" s="0">
-        <v>16.26654633271772</v>
+        <v>15.983216035754685</v>
       </c>
       <c r="D2" s="0">
-        <v>0.4894120140264428</v>
+        <v>0.49258184927264598</v>
       </c>
       <c r="E2" s="0">
-        <v>29.777068859938915</v>
+        <v>31.392631591000779</v>
       </c>
       <c r="F2" s="0">
-        <v>14.515366293396971</v>
+        <v>14.751070143845119</v>
       </c>
       <c r="G2" s="0">
-        <v>0.48746793586945242</v>
+        <v>0.46988956950247396</v>
       </c>
       <c r="H2" s="0">
-        <v>297</v>
+        <v>510.10000000000002</v>
       </c>
       <c r="I2" s="0">
-        <v>263.5</v>
+        <v>479.69999999999993</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>18.666666666666668</v>
+        <v>0.055000000000000007</v>
       </c>
       <c r="B3" s="0">
-        <v>33.295532912991668</v>
+        <v>33.066455269485182</v>
       </c>
       <c r="C3" s="0">
-        <v>16.37153640665068</v>
+        <v>16.156579950853445</v>
       </c>
       <c r="D3" s="0">
-        <v>0.49170369038492334</v>
+        <v>0.48860937222270906</v>
       </c>
       <c r="E3" s="0">
-        <v>29.77974786286434</v>
+        <v>29.433115708657851</v>
       </c>
       <c r="F3" s="0">
-        <v>14.58250857592491</v>
+        <v>14.019504130634449</v>
       </c>
       <c r="G3" s="0">
-        <v>0.48967871195811741</v>
+        <v>0.47631736542626929</v>
       </c>
       <c r="H3" s="0">
-        <v>298.5</v>
+        <v>271.30000000000001</v>
       </c>
       <c r="I3" s="0">
-        <v>265</v>
+        <v>240.10000000000002</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>19</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="B4" s="0">
-        <v>33.187829200973979</v>
+        <v>33.428327833143939</v>
       </c>
       <c r="C4" s="0">
-        <v>16.361864964309575</v>
+        <v>16.04992266498996</v>
       </c>
       <c r="D4" s="0">
-        <v>0.49300798992389039</v>
+        <v>0.48012939041110458</v>
       </c>
       <c r="E4" s="0">
-        <v>29.874797603636665</v>
+        <v>29.85476044020924</v>
       </c>
       <c r="F4" s="0">
-        <v>14.735685327337022</v>
+        <v>14.995006254825931</v>
       </c>
       <c r="G4" s="0">
-        <v>0.49324803879318141</v>
+        <v>0.50226516755533002</v>
       </c>
       <c r="H4" s="0">
-        <v>299.5</v>
+        <v>232.80000000000001</v>
       </c>
       <c r="I4" s="0">
-        <v>266.5</v>
+        <v>203.59999999999997</v>
       </c>
     </row>
     <row r="5">

</xml_diff>